<commit_message>
work on component libraries and schematic
</commit_message>
<xml_diff>
--- a/motor_drive_REV_1/DATASHEETS/BOM.xlsx
+++ b/motor_drive_REV_1/DATASHEETS/BOM.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18312\Desktop\KiCad\motor_drive_REV_1.0\DATASHEETS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18312\Desktop\KiCad\motor_drive\motor_drive_REV_1\DATASHEETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3577F0-F138-4CB3-9950-BE5D7651068F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4426BF76-F2EB-4125-AF01-172054DB0A99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="1185" windowWidth="8685" windowHeight="11850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="1560" windowWidth="6930" windowHeight="12990" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="full list" sheetId="1" r:id="rId1"/>
     <sheet name="top_pick" sheetId="2" r:id="rId2"/>
+    <sheet name="F28027 pin assignment" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>Category</t>
   </si>
@@ -179,6 +180,18 @@
   </si>
   <si>
     <t>ultra</t>
+  </si>
+  <si>
+    <t>FAN7888</t>
+  </si>
+  <si>
+    <t>gate drive B</t>
+  </si>
+  <si>
+    <t>gate drive A</t>
+  </si>
+  <si>
+    <t>PIN</t>
   </si>
 </sst>
 </file>
@@ -740,7 +753,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +907,9 @@
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1092,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4EF55E-36EB-429B-A877-52D9299BE1B0}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,16 +1167,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
         <v>42</v>
@@ -1169,10 +1184,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
@@ -1186,10 +1201,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
@@ -1203,10 +1218,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
@@ -1216,6 +1231,174 @@
       </c>
       <c r="E7" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3082D45B-D41F-4E76-8A53-86D42592906D}">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>